<commit_message>
added template for asset detail
</commit_message>
<xml_diff>
--- a/admin/src/assets/template/Asset_Detail.xlsx
+++ b/admin/src/assets/template/Asset_Detail.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prath\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prath\OneDrive\Desktop\SmartTicket-main\admin\src\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87EC32FC-3FC1-4D45-89CE-30DA21B63E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8571EA54-338C-45A2-B3D8-3B42810A6C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{DC47F645-D363-468B-98CD-0800316B177D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DC47F645-D363-468B-98CD-0800316B177D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Asset Registration Number</t>
   </si>
@@ -58,66 +58,6 @@
   </si>
   <si>
     <t>Permit Exp</t>
-  </si>
-  <si>
-    <t>KA25GF4545</t>
-  </si>
-  <si>
-    <t>KA63R6875</t>
-  </si>
-  <si>
-    <t>KA25GF8788</t>
-  </si>
-  <si>
-    <t>Leyland</t>
-  </si>
-  <si>
-    <t>Tata Motor</t>
-  </si>
-  <si>
-    <t>JLASDJLJO678KSAD</t>
-  </si>
-  <si>
-    <t>JADSDSLN3DA879F</t>
-  </si>
-  <si>
-    <t>LJLDASLLHOE897A</t>
-  </si>
-  <si>
-    <t>79877687SDA089</t>
-  </si>
-  <si>
-    <t>56436252ADA675</t>
-  </si>
-  <si>
-    <t>0899329878DAS3</t>
-  </si>
-  <si>
-    <t>98797989/09</t>
-  </si>
-  <si>
-    <t>68178123/08</t>
-  </si>
-  <si>
-    <t>87877655/01</t>
-  </si>
-  <si>
-    <t>2024-07-12</t>
-  </si>
-  <si>
-    <t>2023-12-25</t>
-  </si>
-  <si>
-    <t>2025-05-31</t>
-  </si>
-  <si>
-    <t>2025-09-15</t>
-  </si>
-  <si>
-    <t>2026-04-20</t>
-  </si>
-  <si>
-    <t>2025-12-18</t>
   </si>
 </sst>
 </file>
@@ -470,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724BB67A-8725-4FFA-9E94-B1CDD866AB4B}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I4" sqref="A2:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,84 +453,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>2012</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>2014</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>2015</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated image signup login page & tickettype fare
</commit_message>
<xml_diff>
--- a/admin/src/assets/template/Asset_Detail.xlsx
+++ b/admin/src/assets/template/Asset_Detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prath\OneDrive\Desktop\SmartTicket-main\admin\src\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8571EA54-338C-45A2-B3D8-3B42810A6C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675F42A4-0ECE-4992-8D9B-41CB3F8C1B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DC47F645-D363-468B-98CD-0800316B177D}"/>
   </bookViews>
@@ -54,10 +54,10 @@
     <t>Permit Number</t>
   </si>
   <si>
-    <t>Insurance Exp</t>
-  </si>
-  <si>
-    <t>Permit Exp</t>
+    <t>Insurance Exp (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Permit Exp (YYYY-MM-DD)</t>
   </si>
 </sst>
 </file>
@@ -95,7 +95,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="A2:I4"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,8 +423,9 @@
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="6" width="17.77734375" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>